<commit_message>
Início CRA - Cesta.
</commit_message>
<xml_diff>
--- a/TSE.xlsx
+++ b/TSE.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20398"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irgpapais\Documents\Meus Projetos\Val\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2650E0-2627-43E1-AADC-61D058C5696D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="8"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="unitario"/>
-    <sheet r:id="rId2" sheetId="2" name="rb"/>
-    <sheet r:id="rId3" sheetId="3" name="NEXEC"/>
-    <sheet r:id="rId4" sheetId="4" name="invest"/>
-    <sheet r:id="rId5" sheetId="5" name="retrabalho"/>
-    <sheet r:id="rId6" sheetId="6" name="n10"/>
-    <sheet r:id="rId7" sheetId="7" name="n3"/>
-    <sheet r:id="rId8" sheetId="8" name="reposicao"/>
-    <sheet r:id="rId9" sheetId="9" name="asfalto"/>
+    <sheet name="unitario" sheetId="1" r:id="rId1"/>
+    <sheet name="rb" sheetId="2" r:id="rId2"/>
+    <sheet name="NEXEC" sheetId="3" r:id="rId3"/>
+    <sheet name="invest" sheetId="4" r:id="rId4"/>
+    <sheet name="retrabalho" sheetId="5" r:id="rId5"/>
+    <sheet name="n10" sheetId="6" r:id="rId6"/>
+    <sheet name="n3" sheetId="7" r:id="rId7"/>
+    <sheet name="reposicao" sheetId="8" r:id="rId8"/>
+    <sheet name="asfalto" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">unitario!$A$1:$C$44</definedName>
   </definedNames>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="268">
   <si>
     <t>731000</t>
   </si>
@@ -823,14 +829,19 @@
   </si>
   <si>
     <t>PRESERVAÇÃO DE INTERFERENCIA INV</t>
+  </si>
+  <si>
+    <t>773000</t>
+  </si>
+  <si>
+    <t>REPOSIÇÃO DE PO ESPECIAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -851,8 +862,23 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -861,7 +887,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92d050"/>
+        <fgColor rgb="FF92D050"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -882,16 +914,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -899,38 +931,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -941,10 +972,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -982,71 +1013,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1074,7 +1105,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1097,11 +1128,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1110,13 +1141,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1126,7 +1157,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1135,7 +1166,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1144,7 +1175,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1152,10 +1183,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1220,7 +1251,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1230,12 +1261,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="45.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="7" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>173</v>
       </c>
@@ -1246,7 +1277,7 @@
         <v>130</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>175</v>
       </c>
@@ -1257,7 +1288,7 @@
         <v>130</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>177</v>
       </c>
@@ -1268,7 +1299,7 @@
         <v>130</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>179</v>
       </c>
@@ -1279,7 +1310,7 @@
         <v>130</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>181</v>
       </c>
@@ -1290,7 +1321,7 @@
         <v>183</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>184</v>
       </c>
@@ -1301,7 +1332,7 @@
         <v>183</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>186</v>
       </c>
@@ -1312,7 +1343,7 @@
         <v>183</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>188</v>
       </c>
@@ -1323,7 +1354,7 @@
         <v>183</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>190</v>
       </c>
@@ -1334,7 +1365,7 @@
         <v>183</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>192</v>
       </c>
@@ -1345,7 +1376,7 @@
         <v>183</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>194</v>
       </c>
@@ -1356,7 +1387,7 @@
         <v>183</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>196</v>
       </c>
@@ -1367,7 +1398,7 @@
         <v>183</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>198</v>
       </c>
@@ -1378,7 +1409,7 @@
         <v>140</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>200</v>
       </c>
@@ -1389,7 +1420,7 @@
         <v>140</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>202</v>
       </c>
@@ -1400,7 +1431,7 @@
         <v>140</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>204</v>
       </c>
@@ -1411,7 +1442,7 @@
         <v>140</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>206</v>
       </c>
@@ -1422,7 +1453,7 @@
         <v>140</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>208</v>
       </c>
@@ -1433,7 +1464,7 @@
         <v>140</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>210</v>
       </c>
@@ -1444,7 +1475,7 @@
         <v>140</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>212</v>
       </c>
@@ -1455,7 +1486,7 @@
         <v>140</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>214</v>
       </c>
@@ -1466,7 +1497,7 @@
         <v>140</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row r="22" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>216</v>
       </c>
@@ -1477,7 +1508,7 @@
         <v>140</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>218</v>
       </c>
@@ -1488,7 +1519,7 @@
         <v>143</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row r="24" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>220</v>
       </c>
@@ -1499,7 +1530,7 @@
         <v>156</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row r="25" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>222</v>
       </c>
@@ -1510,7 +1541,7 @@
         <v>156</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row r="26" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>224</v>
       </c>
@@ -1521,7 +1552,7 @@
         <v>226</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row r="27" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>227</v>
       </c>
@@ -1532,7 +1563,7 @@
         <v>226</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row r="28" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>229</v>
       </c>
@@ -1543,7 +1574,7 @@
         <v>226</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row r="29" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>231</v>
       </c>
@@ -1554,7 +1585,7 @@
         <v>226</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row r="30" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>233</v>
       </c>
@@ -1565,7 +1596,7 @@
         <v>226</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row r="31" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>235</v>
       </c>
@@ -1576,7 +1607,7 @@
         <v>226</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row r="32" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>237</v>
       </c>
@@ -1587,7 +1618,7 @@
         <v>226</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row r="33" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>239</v>
       </c>
@@ -1598,7 +1629,7 @@
         <v>137</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row r="34" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>241</v>
       </c>
@@ -1609,7 +1640,7 @@
         <v>137</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row r="35" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>243</v>
       </c>
@@ -1620,7 +1651,7 @@
         <v>137</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row r="36" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>245</v>
       </c>
@@ -1631,7 +1662,7 @@
         <v>137</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row r="37" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>247</v>
       </c>
@@ -1642,7 +1673,7 @@
         <v>168</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+    <row r="38" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>249</v>
       </c>
@@ -1653,7 +1684,7 @@
         <v>168</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row r="39" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>251</v>
       </c>
@@ -1664,7 +1695,7 @@
         <v>168</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row r="40" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>253</v>
       </c>
@@ -1675,7 +1706,7 @@
         <v>137</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+    <row r="41" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>255</v>
       </c>
@@ -1686,7 +1717,7 @@
         <v>137</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+    <row r="42" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>161</v>
       </c>
@@ -1697,7 +1728,7 @@
         <v>137</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+    <row r="43" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>258</v>
       </c>
@@ -1708,7 +1739,7 @@
         <v>165</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+    <row r="44" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>260</v>
       </c>
@@ -1719,7 +1750,7 @@
         <v>165</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+    <row r="45" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>262</v>
       </c>
@@ -1730,7 +1761,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+    <row r="46" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>264</v>
       </c>
@@ -1741,27 +1772,27 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+    <row r="47" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+    <row r="48" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+    <row r="49" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+    <row r="50" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+    <row r="51" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -1772,55 +1803,57 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="44.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="7" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="9" t="s">
         <v>130</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="9" t="s">
         <v>130</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="9" t="s">
         <v>130</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>135</v>
       </c>
@@ -1831,7 +1864,7 @@
         <v>137</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>138</v>
       </c>
@@ -1842,7 +1875,7 @@
         <v>140</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>141</v>
       </c>
@@ -1853,7 +1886,7 @@
         <v>143</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>144</v>
       </c>
@@ -1864,7 +1897,7 @@
         <v>143</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>146</v>
       </c>
@@ -1875,7 +1908,7 @@
         <v>143</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>148</v>
       </c>
@@ -1886,7 +1919,7 @@
         <v>143</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>150</v>
       </c>
@@ -1897,7 +1930,7 @@
         <v>143</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>152</v>
       </c>
@@ -1908,7 +1941,7 @@
         <v>143</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>154</v>
       </c>
@@ -1919,7 +1952,7 @@
         <v>156</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>157</v>
       </c>
@@ -1930,7 +1963,7 @@
         <v>137</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>159</v>
       </c>
@@ -1941,7 +1974,7 @@
         <v>137</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>161</v>
       </c>
@@ -1952,7 +1985,7 @@
         <v>137</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>163</v>
       </c>
@@ -1963,7 +1996,7 @@
         <v>165</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>166</v>
       </c>
@@ -1974,7 +2007,7 @@
         <v>168</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>169</v>
       </c>
@@ -1985,7 +2018,7 @@
         <v>168</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>171</v>
       </c>
@@ -1998,11 +2031,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2012,11 +2046,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="45.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="7" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.42578125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>72</v>
       </c>
@@ -2024,7 +2058,7 @@
         <v>73</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
@@ -2032,7 +2066,7 @@
         <v>75</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>76</v>
       </c>
@@ -2040,7 +2074,7 @@
         <v>77</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>78</v>
       </c>
@@ -2048,7 +2082,7 @@
         <v>79</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>80</v>
       </c>
@@ -2056,7 +2090,7 @@
         <v>81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>82</v>
       </c>
@@ -2064,7 +2098,7 @@
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>84</v>
       </c>
@@ -2072,7 +2106,7 @@
         <v>85</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>86</v>
       </c>
@@ -2080,7 +2114,7 @@
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>88</v>
       </c>
@@ -2088,7 +2122,7 @@
         <v>89</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>90</v>
       </c>
@@ -2096,7 +2130,7 @@
         <v>91</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>92</v>
       </c>
@@ -2104,7 +2138,7 @@
         <v>93</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>94</v>
       </c>
@@ -2112,7 +2146,7 @@
         <v>95</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>96</v>
       </c>
@@ -2120,7 +2154,7 @@
         <v>97</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>98</v>
       </c>
@@ -2128,7 +2162,7 @@
         <v>99</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>100</v>
       </c>
@@ -2136,7 +2170,7 @@
         <v>101</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>102</v>
       </c>
@@ -2144,7 +2178,7 @@
         <v>103</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>104</v>
       </c>
@@ -2152,7 +2186,7 @@
         <v>105</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>106</v>
       </c>
@@ -2160,7 +2194,7 @@
         <v>107</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>108</v>
       </c>
@@ -2168,7 +2202,7 @@
         <v>109</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>110</v>
       </c>
@@ -2176,7 +2210,7 @@
         <v>111</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>112</v>
       </c>
@@ -2184,7 +2218,7 @@
         <v>113</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row r="22" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>114</v>
       </c>
@@ -2192,7 +2226,7 @@
         <v>115</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row r="23" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>116</v>
       </c>
@@ -2200,7 +2234,7 @@
         <v>117</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row r="24" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>118</v>
       </c>
@@ -2208,7 +2242,7 @@
         <v>119</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row r="25" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>120</v>
       </c>
@@ -2216,7 +2250,7 @@
         <v>121</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row r="26" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>122</v>
       </c>
@@ -2224,7 +2258,7 @@
         <v>123</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row r="27" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>124</v>
       </c>
@@ -2232,7 +2266,7 @@
         <v>125</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row r="28" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>126</v>
       </c>
@@ -2246,7 +2280,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2256,12 +2290,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="25.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="7" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -2278,7 +2312,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2288,11 +2322,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="15.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="7" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>67</v>
       </c>
@@ -2306,40 +2340,46 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="32.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="7" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>63</v>
       </c>
@@ -2350,7 +2390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>65</v>
       </c>
@@ -2367,7 +2407,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2377,12 +2417,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="39.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="7" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
@@ -2393,7 +2433,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>41</v>
       </c>
@@ -2404,7 +2444,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>43</v>
       </c>
@@ -2415,7 +2455,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>45</v>
       </c>
@@ -2426,7 +2466,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>47</v>
       </c>
@@ -2437,7 +2477,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>49</v>
       </c>
@@ -2448,7 +2488,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>51</v>
       </c>
@@ -2459,7 +2499,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>53</v>
       </c>
@@ -2470,7 +2510,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>55</v>
       </c>
@@ -2481,7 +2521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>57</v>
       </c>
@@ -2498,22 +2538,24 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="8.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="44.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2524,7 +2566,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -2535,7 +2577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -2546,7 +2588,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -2557,7 +2599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -2568,7 +2610,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -2579,7 +2621,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -2590,7 +2632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -2601,7 +2643,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -2612,7 +2654,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -2623,7 +2665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -2634,25 +2676,36 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="1" t="s">
+      <c r="C13" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2662,22 +2715,22 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="33.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="7" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2688,7 +2741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2699,7 +2752,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -2710,7 +2763,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -2721,7 +2774,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -2732,7 +2785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Implantação reparo de rede de esgoto.
</commit_message>
<xml_diff>
--- a/TSE.xlsx
+++ b/TSE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irgpapais\Documents\Meus Projetos\Val\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2650E0-2627-43E1-AADC-61D058C5696D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489B5ED3-47E9-4CB5-872E-6A6177782C8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="unitario" sheetId="1" r:id="rId1"/>
@@ -1809,8 +1809,8 @@
   </sheetPr>
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1860,8 +1860,8 @@
       <c r="B4" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>137</v>
+      <c r="C4" s="4" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2346,7 +2346,7 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Implantação de validadores de materiais parte 1.
</commit_message>
<xml_diff>
--- a/TSE.xlsx
+++ b/TSE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irgpapais\Documents\Meus Projetos\Val\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irgpapais\Documents\Meus Projetos\val\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A044AD-6012-4035-8990-D4C25FF70E84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8FA274-27B4-44D5-83C6-4EEB27A2B99A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="unitario" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="293">
   <si>
     <t>731000</t>
   </si>
@@ -904,6 +904,12 @@
   </si>
   <si>
     <t>SONDAGEM DE REDE DE AGUA NÃO VISIVEL</t>
+  </si>
+  <si>
+    <t>714000</t>
+  </si>
+  <si>
+    <t>RETIRADO ENTULHO</t>
   </si>
 </sst>
 </file>
@@ -1980,7 +1986,7 @@
   </sheetPr>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -2745,10 +2751,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2909,6 +2915,17 @@
         <v>38</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Inclusão da União PEAD DN 20 como contratada.
</commit_message>
<xml_diff>
--- a/TSE.xlsx
+++ b/TSE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20399"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20400"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irgpapais\Documents\Meus Projetos\val\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irgpapais\Documents\Meus Projetos\Val\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8FA274-27B4-44D5-83C6-4EEB27A2B99A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C983F59F-E7E0-4093-B92E-7632154C320F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="unitario" sheetId="1" r:id="rId1"/>
@@ -24,14 +24,14 @@
     <sheet name="asfalto" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">unitario!$A$4:$C$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">unitario!$A$4:$C$54</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="295">
   <si>
     <t>731000</t>
   </si>
@@ -910,6 +910,12 @@
   </si>
   <si>
     <t>RETIRADO ENTULHO</t>
+  </si>
+  <si>
+    <t>322000</t>
+  </si>
+  <si>
+    <t>TROCA DE CAIXA DE PARADA</t>
   </si>
 </sst>
 </file>
@@ -1330,9 +1336,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -1664,32 +1670,32 @@
     </row>
     <row r="30" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>284</v>
+        <v>220</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>283</v>
+        <v>221</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>156</v>
@@ -1697,10 +1703,10 @@
     </row>
     <row r="33" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>156</v>
@@ -1708,10 +1714,10 @@
     </row>
     <row r="34" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>222</v>
+        <v>281</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>223</v>
+        <v>282</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>156</v>
@@ -1719,21 +1725,21 @@
     </row>
     <row r="35" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>226</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>226</v>
@@ -1741,10 +1747,10 @@
     </row>
     <row r="37" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>226</v>
@@ -1752,10 +1758,10 @@
     </row>
     <row r="38" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>226</v>
@@ -1763,10 +1769,10 @@
     </row>
     <row r="39" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>226</v>
@@ -1774,10 +1780,10 @@
     </row>
     <row r="40" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>226</v>
@@ -1785,32 +1791,32 @@
     </row>
     <row r="41" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>137</v>
+      <c r="A42" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>137</v>
@@ -1818,10 +1824,10 @@
     </row>
     <row r="44" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>137</v>
@@ -1829,10 +1835,10 @@
     </row>
     <row r="45" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>137</v>
@@ -1840,21 +1846,21 @@
     </row>
     <row r="46" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>168</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>168</v>
@@ -1862,10 +1868,10 @@
     </row>
     <row r="48" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>168</v>
@@ -1873,21 +1879,21 @@
     </row>
     <row r="49" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>137</v>
+        <v>168</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>137</v>
@@ -1895,10 +1901,10 @@
     </row>
     <row r="51" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>161</v>
+        <v>255</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>137</v>
@@ -1906,21 +1912,21 @@
     </row>
     <row r="52" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>258</v>
+        <v>161</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>165</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>165</v>
@@ -1928,30 +1934,36 @@
     </row>
     <row r="54" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>2</v>
+        <v>165</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="7"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
+      <c r="C56" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="57" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
@@ -1972,6 +1984,11 @@
       <c r="A60" s="7"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
+    </row>
+    <row r="61" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="7"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2753,7 +2770,7 @@
   </sheetPr>
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
inclusão da png água.
</commit_message>
<xml_diff>
--- a/TSE.xlsx
+++ b/TSE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irgpapais\Documents\Meus Projetos\val\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5EA369-3837-4A86-AAEB-91B9A3C1B018}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC3A924-5A41-4A44-9E69-2001CB2750B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="unitario" sheetId="1" r:id="rId1"/>
@@ -24,14 +24,14 @@
     <sheet name="asfalto" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">unitario!$A$4:$C$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">unitario!$A$4:$C$55</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="293">
   <si>
     <t>731000</t>
   </si>
@@ -904,6 +904,12 @@
   </si>
   <si>
     <t>TROCA DE CAIXA DE PARADA</t>
+  </si>
+  <si>
+    <t>280000</t>
+  </si>
+  <si>
+    <t>PASSADO RAMAL DE AGUA PARA NOVA REDE</t>
   </si>
 </sst>
 </file>
@@ -1000,7 +1006,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1019,6 +1025,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1324,10 +1331,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1625,21 +1632,21 @@
     </row>
     <row r="27" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C27" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>136</v>
@@ -1647,54 +1654,54 @@
     </row>
     <row r="29" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>164</v>
+        <v>214</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>280</v>
+        <v>216</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>279</v>
+        <v>217</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>152</v>
@@ -1702,10 +1709,10 @@
     </row>
     <row r="34" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>152</v>
@@ -1713,10 +1720,10 @@
     </row>
     <row r="35" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>218</v>
+        <v>277</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>219</v>
+        <v>278</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>152</v>
@@ -1724,21 +1731,21 @@
     </row>
     <row r="36" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>222</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>222</v>
@@ -1746,10 +1753,10 @@
     </row>
     <row r="38" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>222</v>
@@ -1757,10 +1764,10 @@
     </row>
     <row r="39" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>222</v>
@@ -1768,10 +1775,10 @@
     </row>
     <row r="40" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>222</v>
@@ -1779,10 +1786,10 @@
     </row>
     <row r="41" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>222</v>
@@ -1790,32 +1797,32 @@
     </row>
     <row r="42" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>133</v>
+      <c r="A43" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>133</v>
@@ -1823,10 +1830,10 @@
     </row>
     <row r="45" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>133</v>
@@ -1834,10 +1841,10 @@
     </row>
     <row r="46" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>133</v>
@@ -1845,21 +1852,21 @@
     </row>
     <row r="47" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>164</v>
@@ -1867,10 +1874,10 @@
     </row>
     <row r="49" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>164</v>
@@ -1878,21 +1885,21 @@
     </row>
     <row r="50" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>133</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>133</v>
@@ -1900,10 +1907,10 @@
     </row>
     <row r="52" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>157</v>
+        <v>251</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>133</v>
@@ -1911,21 +1918,21 @@
     </row>
     <row r="53" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>254</v>
+        <v>157</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>161</v>
@@ -1933,30 +1940,36 @@
     </row>
     <row r="55" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>2</v>
+        <v>161</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="7"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
+      <c r="C57" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="58" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
@@ -1977,6 +1990,11 @@
       <c r="A61" s="7"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
+    </row>
+    <row r="62" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="7"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2560,7 +2578,7 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Inclusão do localizador e mesclagem materiais de água.
</commit_message>
<xml_diff>
--- a/TSE.xlsx
+++ b/TSE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irgpapais\Documents\Meus Projetos\val\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC3A924-5A41-4A44-9E69-2001CB2750B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6867708-3E4C-45BF-B3A4-ED4F023BE94B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,14 +24,14 @@
     <sheet name="asfalto" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">unitario!$A$4:$C$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">unitario!$A$4:$C$56</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="295">
   <si>
     <t>731000</t>
   </si>
@@ -910,6 +910,12 @@
   </si>
   <si>
     <t>PASSADO RAMAL DE AGUA PARA NOVA REDE</t>
+  </si>
+  <si>
+    <t>312000</t>
+  </si>
+  <si>
+    <t>NIVELADA CAIXA DE PARADA</t>
   </si>
 </sst>
 </file>
@@ -1331,10 +1337,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1676,10 +1682,10 @@
     </row>
     <row r="31" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>164</v>
@@ -1687,32 +1693,32 @@
     </row>
     <row r="32" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>280</v>
+        <v>216</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>279</v>
+        <v>217</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>152</v>
@@ -1720,10 +1726,10 @@
     </row>
     <row r="35" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>152</v>
@@ -1731,10 +1737,10 @@
     </row>
     <row r="36" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>218</v>
+        <v>277</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>219</v>
+        <v>278</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>152</v>
@@ -1742,21 +1748,21 @@
     </row>
     <row r="37" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>222</v>
+        <v>152</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>222</v>
@@ -1764,10 +1770,10 @@
     </row>
     <row r="39" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>222</v>
@@ -1775,10 +1781,10 @@
     </row>
     <row r="40" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>222</v>
@@ -1786,10 +1792,10 @@
     </row>
     <row r="41" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>222</v>
@@ -1797,10 +1803,10 @@
     </row>
     <row r="42" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>222</v>
@@ -1808,32 +1814,32 @@
     </row>
     <row r="43" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>133</v>
+      <c r="A44" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>133</v>
@@ -1841,10 +1847,10 @@
     </row>
     <row r="46" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>133</v>
@@ -1852,10 +1858,10 @@
     </row>
     <row r="47" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>133</v>
@@ -1863,21 +1869,21 @@
     </row>
     <row r="48" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>164</v>
@@ -1885,10 +1891,10 @@
     </row>
     <row r="50" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>164</v>
@@ -1896,21 +1902,21 @@
     </row>
     <row r="51" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>133</v>
+        <v>164</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>133</v>
@@ -1918,10 +1924,10 @@
     </row>
     <row r="53" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>157</v>
+        <v>251</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>133</v>
@@ -1929,21 +1935,21 @@
     </row>
     <row r="54" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>254</v>
+        <v>157</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>161</v>
@@ -1951,30 +1957,36 @@
     </row>
     <row r="56" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>2</v>
+        <v>161</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="7"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
+      <c r="C58" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="59" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
@@ -1995,6 +2007,11 @@
       <c r="A62" s="7"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
+    </row>
+    <row r="63" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="7"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Correção materiais água, proibidos e tses novas.
</commit_message>
<xml_diff>
--- a/TSE.xlsx
+++ b/TSE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20403"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irgpapais\Documents\Meus Projetos\val\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irgpapais\Documents\Meus Projetos\Val\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6867708-3E4C-45BF-B3A4-ED4F023BE94B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412BEE4C-15AC-4D2E-AA1F-DD9AAF7DE7A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="unitario" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="asfalto" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">unitario!$A$4:$C$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">unitario!$A$3:$C$55</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -1337,10 +1337,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1372,23 +1372,23 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="C3" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>126</v>
@@ -1396,10 +1396,10 @@
     </row>
     <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>126</v>
@@ -1407,10 +1407,10 @@
     </row>
     <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>126</v>
@@ -1418,32 +1418,32 @@
     </row>
     <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C7" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>126</v>
+      <c r="A8" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>177</v>
+        <v>265</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>178</v>
+        <v>266</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>179</v>
@@ -1451,10 +1451,10 @@
     </row>
     <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>265</v>
+        <v>180</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>266</v>
+        <v>181</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>179</v>
@@ -1462,10 +1462,10 @@
     </row>
     <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>179</v>
@@ -1473,10 +1473,10 @@
     </row>
     <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>179</v>
@@ -1484,10 +1484,10 @@
     </row>
     <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>179</v>
@@ -1495,10 +1495,10 @@
     </row>
     <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>179</v>
@@ -1506,10 +1506,10 @@
     </row>
     <row r="15" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>179</v>
@@ -1517,10 +1517,10 @@
     </row>
     <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>190</v>
+        <v>275</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>191</v>
+        <v>276</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>179</v>
@@ -1528,32 +1528,32 @@
     </row>
     <row r="17" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>275</v>
+        <v>192</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>276</v>
+        <v>193</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>179</v>
+      <c r="A18" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>136</v>
@@ -1561,10 +1561,10 @@
     </row>
     <row r="20" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>136</v>
@@ -1572,10 +1572,10 @@
     </row>
     <row r="21" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>136</v>
@@ -1583,10 +1583,10 @@
     </row>
     <row r="22" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>136</v>
@@ -1594,10 +1594,10 @@
     </row>
     <row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>136</v>
@@ -1605,10 +1605,10 @@
     </row>
     <row r="24" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>136</v>
@@ -1616,10 +1616,10 @@
     </row>
     <row r="25" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>136</v>
@@ -1627,32 +1627,32 @@
     </row>
     <row r="26" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="C26" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="C26" s="10" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>292</v>
-      </c>
-      <c r="C27" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>136</v>
@@ -1660,32 +1660,32 @@
     </row>
     <row r="29" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>139</v>
+        <v>293</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>164</v>
@@ -1693,32 +1693,32 @@
     </row>
     <row r="32" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>164</v>
+        <v>142</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>139</v>
+      <c r="A33" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>216</v>
+        <v>280</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>217</v>
+        <v>279</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>152</v>
@@ -1726,10 +1726,10 @@
     </row>
     <row r="35" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>152</v>
@@ -1737,10 +1737,10 @@
     </row>
     <row r="36" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>277</v>
+        <v>218</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>278</v>
+        <v>219</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>152</v>
@@ -1748,21 +1748,21 @@
     </row>
     <row r="37" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>152</v>
+        <v>222</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>222</v>
@@ -1770,10 +1770,10 @@
     </row>
     <row r="39" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>222</v>
@@ -1781,10 +1781,10 @@
     </row>
     <row r="40" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>222</v>
@@ -1792,10 +1792,10 @@
     </row>
     <row r="41" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>222</v>
@@ -1803,10 +1803,10 @@
     </row>
     <row r="42" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>222</v>
@@ -1814,32 +1814,32 @@
     </row>
     <row r="43" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>222</v>
+      <c r="A44" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>133</v>
@@ -1847,10 +1847,10 @@
     </row>
     <row r="46" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>133</v>
@@ -1858,10 +1858,10 @@
     </row>
     <row r="47" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>133</v>
@@ -1869,21 +1869,21 @@
     </row>
     <row r="48" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>133</v>
+        <v>164</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>164</v>
@@ -1891,10 +1891,10 @@
     </row>
     <row r="50" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>164</v>
@@ -1902,21 +1902,21 @@
     </row>
     <row r="51" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>133</v>
@@ -1924,10 +1924,10 @@
     </row>
     <row r="53" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>251</v>
+        <v>157</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>133</v>
@@ -1935,21 +1935,21 @@
     </row>
     <row r="54" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>157</v>
+        <v>254</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>161</v>
@@ -1957,36 +1957,30 @@
     </row>
     <row r="56" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>161</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A58" s="7"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
     </row>
     <row r="59" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
@@ -2007,11 +2001,6 @@
       <c r="A62" s="7"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
-    </row>
-    <row r="63" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="7"/>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2024,10 +2013,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2050,10 +2039,10 @@
     </row>
     <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>127</v>
+        <v>274</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>128</v>
+        <v>273</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>126</v>
@@ -2061,32 +2050,32 @@
     </row>
     <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>136</v>
+      <c r="A4" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>284</v>
+        <v>131</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>136</v>
@@ -2094,65 +2083,65 @@
     </row>
     <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C6" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>282</v>
-      </c>
-      <c r="C7" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>139</v>
+        <v>281</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="C9" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C10" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>139</v>
@@ -2160,10 +2149,10 @@
     </row>
     <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>139</v>
@@ -2171,10 +2160,10 @@
     </row>
     <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>139</v>
@@ -2182,32 +2171,32 @@
     </row>
     <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>133</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>133</v>
@@ -2215,10 +2204,10 @@
     </row>
     <row r="17" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>133</v>
@@ -2226,32 +2215,32 @@
     </row>
     <row r="18" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>164</v>
@@ -2259,12 +2248,23 @@
     </row>
     <row r="21" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>161</v>
       </c>
     </row>
@@ -2525,7 +2525,9 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
materiais esgoto, pendentes excel.
</commit_message>
<xml_diff>
--- a/TSE.xlsx
+++ b/TSE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20403"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20404"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irgpapais\Documents\Meus Projetos\Val\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412BEE4C-15AC-4D2E-AA1F-DD9AAF7DE7A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F570C16-CD33-4136-995F-AA5992BB5B76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="unitario" sheetId="1" r:id="rId1"/>
@@ -24,14 +24,14 @@
     <sheet name="asfalto" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">unitario!$A$3:$C$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">unitario!$A$3:$C$56</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="297">
   <si>
     <t>731000</t>
   </si>
@@ -916,6 +916,12 @@
   </si>
   <si>
     <t>NIVELADA CAIXA DE PARADA</t>
+  </si>
+  <si>
+    <t>SUBSTITUIDA LIGAÇÃO DE AGUA DIMENSIONADA</t>
+  </si>
+  <si>
+    <t>263000</t>
   </si>
 </sst>
 </file>
@@ -1337,10 +1343,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1583,21 +1589,21 @@
     </row>
     <row r="22" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="C22" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>136</v>
@@ -1605,10 +1611,10 @@
     </row>
     <row r="24" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>136</v>
@@ -1616,10 +1622,10 @@
     </row>
     <row r="25" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>136</v>
@@ -1627,32 +1633,32 @@
     </row>
     <row r="26" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>292</v>
-      </c>
-      <c r="C26" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C27" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>136</v>
@@ -1660,32 +1666,32 @@
     </row>
     <row r="29" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>164</v>
+        <v>214</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>164</v>
@@ -1693,32 +1699,32 @@
     </row>
     <row r="32" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>280</v>
+        <v>216</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>279</v>
+        <v>217</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>152</v>
@@ -1726,10 +1732,10 @@
     </row>
     <row r="35" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>152</v>
@@ -1737,10 +1743,10 @@
     </row>
     <row r="36" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>218</v>
+        <v>277</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>219</v>
+        <v>278</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>152</v>
@@ -1748,21 +1754,21 @@
     </row>
     <row r="37" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>222</v>
+        <v>152</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>222</v>
@@ -1770,10 +1776,10 @@
     </row>
     <row r="39" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>222</v>
@@ -1781,10 +1787,10 @@
     </row>
     <row r="40" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>222</v>
@@ -1792,10 +1798,10 @@
     </row>
     <row r="41" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>222</v>
@@ -1803,10 +1809,10 @@
     </row>
     <row r="42" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>222</v>
@@ -1814,32 +1820,32 @@
     </row>
     <row r="43" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>133</v>
+      <c r="A44" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>133</v>
@@ -1847,10 +1853,10 @@
     </row>
     <row r="46" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>133</v>
@@ -1858,10 +1864,10 @@
     </row>
     <row r="47" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>133</v>
@@ -1869,21 +1875,21 @@
     </row>
     <row r="48" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>164</v>
@@ -1891,10 +1897,10 @@
     </row>
     <row r="50" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>164</v>
@@ -1902,21 +1908,21 @@
     </row>
     <row r="51" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>133</v>
+        <v>164</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>133</v>
@@ -1924,10 +1930,10 @@
     </row>
     <row r="53" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>157</v>
+        <v>251</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>133</v>
@@ -1935,21 +1941,21 @@
     </row>
     <row r="54" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>254</v>
+        <v>157</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>161</v>
@@ -1957,30 +1963,36 @@
     </row>
     <row r="56" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>2</v>
+        <v>161</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="7"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
+      <c r="C58" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="59" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
@@ -2001,6 +2013,11 @@
       <c r="A62" s="7"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
+    </row>
+    <row r="63" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="7"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2015,8 +2032,8 @@
   </sheetPr>
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>